<commit_message>
New API Query - 2023 Included
API query to UN performed 11/26/2023.
Query modified to include 2023 data.
</commit_message>
<xml_diff>
--- a/Excel-XLSX/UN-ANT.xlsx
+++ b/Excel-XLSX/UN-ANT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>﻿"page"</t>
   </si>
@@ -87,7 +87,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>1Qt1OM</t>
+    <t>4zcdNp</t>
   </si>
   <si>
     <t>2007</t>
@@ -120,7 +120,37 @@
     <t>5</t>
   </si>
   <si>
-    <t>null</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>HAI</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>2015</t>
@@ -138,31 +168,10 @@
     <t>15</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>2016</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>Haiti</t>
-  </si>
-  <si>
-    <t>HAI</t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
-    <t>36</t>
+    <t>6</t>
   </si>
   <si>
     <t>207</t>
@@ -174,7 +183,10 @@
     <t>VEN</t>
   </si>
   <si>
-    <t>59</t>
+    <t>54</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
 </sst>
 </file>
@@ -559,7 +571,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -699,8 +711,8 @@
       <c r="U2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>32</v>
+      <c r="V2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -729,7 +741,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>28</v>
@@ -744,7 +756,7 @@
         <v>31</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>32</v>
@@ -762,7 +774,7 @@
         <v>32</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>34</v>
@@ -782,10 +794,10 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>36</v>
@@ -797,7 +809,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>28</v>
@@ -812,7 +824,7 @@
         <v>31</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>32</v>
@@ -830,7 +842,7 @@
         <v>32</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>34</v>
@@ -850,22 +862,22 @@
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>28</v>
@@ -880,7 +892,7 @@
         <v>31</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>32</v>
@@ -898,13 +910,13 @@
         <v>32</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="2" t="s">
-        <v>32</v>
+      <c r="V5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -921,19 +933,19 @@
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>28</v>
@@ -948,7 +960,7 @@
         <v>31</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>32</v>
@@ -966,12 +978,148 @@
         <v>32</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="V6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>